<commit_message>
create good page modified
</commit_message>
<xml_diff>
--- a/activity.xlsx
+++ b/activity.xlsx
@@ -75,24 +75,6 @@
     <t>получено</t>
   </si>
   <si>
-    <t>Ручка переключения передач spaco (сереб-черн-кр)</t>
-  </si>
-  <si>
-    <t>Ручка переключения кпп SPACO (сереб - черн - кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
-  </si>
-  <si>
-    <t>Ручка переключения передач spaco (сереб - черн)</t>
-  </si>
-  <si>
-    <t>Ручка переключения передач spaco (черн - бел)</t>
-  </si>
-  <si>
-    <t>Ручка переключения передач spaco (черн - бел - кр)</t>
-  </si>
-  <si>
-    <t>Ручка переключения передач spaco (черн-кр)</t>
-  </si>
-  <si>
     <t>Ручка переключения передач mugen (кр)</t>
   </si>
   <si>
@@ -103,18 +85,6 @@
   </si>
   <si>
     <t>Ручка переключения кпп MOMO (кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
-  </si>
-  <si>
-    <t>Ручка переключения кпп spaco (сереб - черн), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
-  </si>
-  <si>
-    <t>Ручка переключения кпп spaco (черн - бел), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
-  </si>
-  <si>
-    <t>Ручка переключения кпп spaco (черн - бел - кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
-  </si>
-  <si>
-    <t>Ручка переключения кпп spaco (черн-кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
   </si>
   <si>
     <t>Накладки на педали Ford Focus, Мondeo (мкпп)</t>
@@ -241,6 +211,36 @@
   </si>
   <si>
     <t>Skoda/VW</t>
+  </si>
+  <si>
+    <t>Ручка переключения передач sparco (сереб-черн-кр)</t>
+  </si>
+  <si>
+    <t>Ручка переключения передач sparco (сереб - черн)</t>
+  </si>
+  <si>
+    <t>Ручка переключения передач sparco (черн - бел)</t>
+  </si>
+  <si>
+    <t>Ручка переключения передач sparco (черн - бел - кр)</t>
+  </si>
+  <si>
+    <t>Ручка переключения передач sparco (черн-кр)</t>
+  </si>
+  <si>
+    <t>Ручка переключения кпп SPARCO (сереб - черн - кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
+  </si>
+  <si>
+    <t>Ручка переключения кпп SPARCO (сереб - черн), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
+  </si>
+  <si>
+    <t>Ручка переключения кпп SPARCO (черн - бел), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
+  </si>
+  <si>
+    <t>Ручка переключения кпп SPARCO (черн - бел - кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
+  </si>
+  <si>
+    <t>Ручка переключения кпп SPARCO (черн-кр), в комплекте переходные гайки под разную резьбу штока - M8/М10/M12</t>
   </si>
 </sst>
 </file>
@@ -687,7 +687,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,18 +728,18 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>10</v>
@@ -754,11 +754,11 @@
         <v>3300</v>
       </c>
       <c r="F2" s="5">
-        <f>(E2-D2)/D2*100</f>
+        <f t="shared" ref="F2:F11" si="0">(E2-D2)/D2*100</f>
         <v>83.93008427342042</v>
       </c>
       <c r="G2" s="5">
-        <f>E2-D2</f>
+        <f t="shared" ref="G2:G11" si="1">E2-D2</f>
         <v>1505.84</v>
       </c>
       <c r="H2" s="5"/>
@@ -785,11 +785,11 @@
         <v>3300</v>
       </c>
       <c r="F3" s="5">
-        <f>(E3-D3)/D3*100</f>
+        <f t="shared" si="0"/>
         <v>103.41365090519075</v>
       </c>
       <c r="G3" s="5">
-        <f>E3-D3</f>
+        <f t="shared" si="1"/>
         <v>1677.69</v>
       </c>
       <c r="H3" s="5"/>
@@ -801,13 +801,13 @@
     </row>
     <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -816,11 +816,11 @@
         <v>2200</v>
       </c>
       <c r="F4" s="5">
-        <f>(E4-D4)/D4*100</f>
+        <f t="shared" si="0"/>
         <v>219900</v>
       </c>
       <c r="G4" s="5">
-        <f>E4-D4</f>
+        <f t="shared" si="1"/>
         <v>2199</v>
       </c>
       <c r="H4" s="5"/>
@@ -832,10 +832,10 @@
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -844,11 +844,11 @@
         <v>2200</v>
       </c>
       <c r="F5" s="5">
-        <f>(E5-D5)/D5*100</f>
+        <f t="shared" si="0"/>
         <v>219900</v>
       </c>
       <c r="G5" s="5">
-        <f>E5-D5</f>
+        <f t="shared" si="1"/>
         <v>2199</v>
       </c>
       <c r="H5" s="5"/>
@@ -860,13 +860,13 @@
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -875,11 +875,11 @@
         <v>2200</v>
       </c>
       <c r="F6" s="7">
-        <f>(E6-D6)/D6*100</f>
+        <f t="shared" si="0"/>
         <v>219900</v>
       </c>
       <c r="G6" s="7">
-        <f>E6-D6</f>
+        <f t="shared" si="1"/>
         <v>2199</v>
       </c>
       <c r="H6" s="7"/>
@@ -889,16 +889,16 @@
         <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D7" s="11">
         <v>1</v>
@@ -907,11 +907,11 @@
         <v>2200</v>
       </c>
       <c r="F7" s="12">
-        <f>(E7-D7)/D7*100</f>
+        <f t="shared" si="0"/>
         <v>219900</v>
       </c>
       <c r="G7" s="12">
-        <f>E7-D7</f>
+        <f t="shared" si="1"/>
         <v>2199</v>
       </c>
       <c r="H7" s="12"/>
@@ -921,18 +921,18 @@
         <v>0</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D8" s="6">
         <v>576.41999999999996</v>
@@ -941,11 +941,11 @@
         <v>1</v>
       </c>
       <c r="F8" s="7">
-        <f>(E8-D8)/D8*100</f>
+        <f t="shared" si="0"/>
         <v>-99.826515388085085</v>
       </c>
       <c r="G8" s="7">
-        <f>E8-D8</f>
+        <f t="shared" si="1"/>
         <v>-575.41999999999996</v>
       </c>
       <c r="H8" s="7"/>
@@ -955,18 +955,18 @@
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -975,11 +975,11 @@
         <v>2200</v>
       </c>
       <c r="F9" s="7">
-        <f>(E9-D9)/D9*100</f>
+        <f t="shared" si="0"/>
         <v>219900</v>
       </c>
       <c r="G9" s="7">
-        <f>E9-D9</f>
+        <f t="shared" si="1"/>
         <v>2199</v>
       </c>
       <c r="H9" s="7"/>
@@ -989,18 +989,18 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D10" s="6">
         <v>1067.5</v>
@@ -1009,11 +1009,11 @@
         <v>2200</v>
       </c>
       <c r="F10" s="7">
-        <f>(E10-D10)/D10*100</f>
+        <f t="shared" si="0"/>
         <v>106.08899297423888</v>
       </c>
       <c r="G10" s="7">
-        <f>E10-D10</f>
+        <f t="shared" si="1"/>
         <v>1132.5</v>
       </c>
       <c r="H10" s="7"/>
@@ -1023,32 +1023,32 @@
         <v>2</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D11" s="6">
-        <v>1756.85</v>
+        <v>1021.96</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
       </c>
       <c r="F11" s="7">
-        <f>(E11-D11)/D11*100</f>
-        <v>-99.943079944218354</v>
+        <f t="shared" si="0"/>
+        <v>-99.90214881208658</v>
       </c>
       <c r="G11" s="7">
-        <f>E11-D11</f>
-        <v>-1755.85</v>
+        <f t="shared" si="1"/>
+        <v>-1020.96</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1108,24 +1108,24 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4">
         <v>860.67</v>
@@ -1155,13 +1155,13 @@
     </row>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4">
         <v>2512.37</v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="4" spans="1:12" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D4" s="16">
         <v>1</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D5" s="6">
         <v>897.27</v>
@@ -1250,18 +1250,18 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D6" s="6">
         <v>1614.89</v>
@@ -1284,12 +1284,12 @@
         <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="17">
@@ -1298,7 +1298,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17">
@@ -1307,7 +1307,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="K9" s="17">
         <v>0</v>
@@ -1323,7 +1323,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,21 +1358,21 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1400,12 +1400,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -1435,10 +1435,10 @@
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
@@ -1468,10 +1468,10 @@
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1534,10 +1534,10 @@
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -1567,10 +1567,10 @@
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>

</xml_diff>